<commit_message>
add download template feature
</commit_message>
<xml_diff>
--- a/downloads/hr/Raw database.xlsx
+++ b/downloads/hr/Raw database.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiangy2o\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiangy2o\OneDrive\Documents\root\dev\src\trust-app\downloads\hr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B309B6-2105-49F9-9F04-45783BB812BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A92012F-D9DF-4FFF-BD25-96AB80071326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78F82434-1DE3-4928-B2E7-C0B05132959C}"/>
   </bookViews>
@@ -280,6 +280,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -582,7 +586,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update the import excel template
</commit_message>
<xml_diff>
--- a/downloads/hr/Raw database.xlsx
+++ b/downloads/hr/Raw database.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiangy2o\OneDrive\Documents\root\dev\src\trust-app\downloads\hr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiangy2o\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A92012F-D9DF-4FFF-BD25-96AB80071326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1EA4BD-DEE8-4E3D-AD85-532715FF8838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{78F82434-1DE3-4928-B2E7-C0B05132959C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>S.no</t>
   </si>
@@ -108,18 +108,9 @@
     <t xml:space="preserve">Reason for Leaving </t>
   </si>
   <si>
-    <t xml:space="preserve"> PA Corporate Management Portfolio</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>12/22/2024</t>
-  </si>
-  <si>
     <t>Volunteer</t>
   </si>
   <si>
@@ -138,9 +129,6 @@
     <t>100 Spring Rd, Auckland</t>
   </si>
   <si>
-    <t>06/23/1991</t>
-  </si>
-  <si>
     <t>New Zealand</t>
   </si>
   <si>
@@ -153,16 +141,37 @@
     <t>This is a comment</t>
   </si>
   <si>
-    <t>01/14/2025</t>
-  </si>
-  <si>
-    <t>01/20/2025</t>
-  </si>
-  <si>
     <t>relocation</t>
   </si>
   <si>
     <t>excellent</t>
+  </si>
+  <si>
+    <t>John Smith 2</t>
+  </si>
+  <si>
+    <t>John Smith 3</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Hybrid</t>
+  </si>
+  <si>
+    <t>Remote</t>
+  </si>
+  <si>
+    <t>PA Corporate Management Portfolio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Development Management Portfolio </t>
+  </si>
+  <si>
+    <t>Events - Co- ordinator Management Portfolio (open)</t>
   </si>
 </sst>
 </file>
@@ -191,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +216,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -239,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -253,6 +268,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -280,10 +298,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -583,23 +597,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2640DA58-EBC9-49DA-84FC-C1712E2E8B86}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="20" style="4"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="20" style="4"/>
     <col min="11" max="11" width="46.140625" customWidth="1"/>
+    <col min="14" max="14" width="20" style="4"/>
+    <col min="21" max="22" width="20" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="2" customFormat="1" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -608,7 +626,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -635,7 +653,7 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
@@ -656,10 +674,10 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="7" t="s">
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
@@ -673,80 +691,218 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
-        <v>45633</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="4">
+        <v>45648</v>
+      </c>
+      <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" t="s">
         <v>29</v>
       </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
+      <c r="N2" s="4">
+        <v>45831</v>
+      </c>
+      <c r="O2" t="s">
         <v>31</v>
       </c>
-      <c r="J2">
-        <v>40</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="P2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N2" t="s">
+      <c r="S2" t="s">
         <v>34</v>
-      </c>
-      <c r="O2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" t="s">
-        <v>38</v>
       </c>
       <c r="T2">
         <v>3</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="4">
+        <v>45671</v>
+      </c>
+      <c r="V2" s="4">
+        <v>42024</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4">
+        <v>45648</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="4">
+        <v>45831</v>
+      </c>
+      <c r="O3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3">
+        <v>3</v>
+      </c>
+      <c r="U3" s="4">
+        <v>45671</v>
+      </c>
+      <c r="V3" s="4">
+        <v>42024</v>
+      </c>
+      <c r="W3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>45204</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
         <v>39</v>
       </c>
-      <c r="V2" t="s">
+      <c r="E4" s="4">
+        <v>45648</v>
+      </c>
+      <c r="F4" t="s">
         <v>40</v>
       </c>
-      <c r="W2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
         <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="4">
+        <v>45831</v>
+      </c>
+      <c r="O4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T4">
+        <v>3</v>
+      </c>
+      <c r="U4" s="4">
+        <v>45671</v>
+      </c>
+      <c r="V4" s="4">
+        <v>42024</v>
+      </c>
+      <c r="W4" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{D0010353-2DB8-4FE5-A21A-97A97C83627C}">
+      <formula1>"Male,Female"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{A34657F8-7851-4882-B648-B03495ADAEEB}">
+      <formula1>"Employee,Volunteer"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{C281D9C8-51CA-4278-BE24-79ACBDF03B79}">
+      <formula1>"Onsite,Remote,Hybrid"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="Q2" r:id="rId1" xr:uid="{044FF3CC-63E3-4A21-B514-A7CCDBDC5D50}"/>
+    <hyperlink ref="Q3" r:id="rId2" xr:uid="{3B2C356C-17B4-4850-9589-B3A3EBD76A90}"/>
+    <hyperlink ref="Q4" r:id="rId3" xr:uid="{5DAADB1B-8988-478A-BF44-6D32F9504D7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>